<commit_message>
excel demo and some other classes added
</commit_message>
<xml_diff>
--- a/src/test/resources/LoginList.xlsx
+++ b/src/test/resources/LoginList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDDC64FF-9CF0-42BF-BF4C-A6328FF8CD38}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320138F8-39F3-4810-AE85-4B7E90B760C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1155" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1155" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QaTeam1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="49">
   <si>
     <t>Your Name</t>
   </si>
@@ -102,6 +102,78 @@
   </si>
   <si>
     <t>sg12345678</t>
+  </si>
+  <si>
+    <t>okul</t>
+  </si>
+  <si>
+    <t>degree</t>
+  </si>
+  <si>
+    <t>study</t>
+  </si>
+  <si>
+    <t>fromdate</t>
+  </si>
+  <si>
+    <t>Todate</t>
+  </si>
+  <si>
+    <t>Program Desc</t>
+  </si>
+  <si>
+    <t>gazi</t>
+  </si>
+  <si>
+    <t>otdü</t>
+  </si>
+  <si>
+    <t>bilkent</t>
+  </si>
+  <si>
+    <t>ege</t>
+  </si>
+  <si>
+    <t>itü</t>
+  </si>
+  <si>
+    <t>ktü</t>
+  </si>
+  <si>
+    <t>yildiz</t>
+  </si>
+  <si>
+    <t>istanbul</t>
+  </si>
+  <si>
+    <t>ankara</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>nice</t>
+  </si>
+  <si>
+    <t>very good</t>
+  </si>
+  <si>
+    <t>finance</t>
+  </si>
+  <si>
+    <t>medical</t>
+  </si>
+  <si>
+    <t>engineer</t>
+  </si>
+  <si>
+    <t>Nice Program</t>
+  </si>
+  <si>
+    <t>Excellent Program</t>
+  </si>
+  <si>
+    <t>Not Bad program</t>
   </si>
 </sst>
 </file>
@@ -464,7 +536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -807,10 +879,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8D8DB64-3C2D-4923-B33A-9078A63670CF}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -818,9 +890,12 @@
     <col min="1" max="1" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -830,8 +905,26 @@
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -841,8 +934,26 @@
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2">
+        <v>11122021</v>
+      </c>
+      <c r="H2">
+        <v>12122022</v>
+      </c>
+      <c r="I2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -852,8 +963,26 @@
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3">
+        <v>11122020</v>
+      </c>
+      <c r="H3">
+        <v>12122022</v>
+      </c>
+      <c r="I3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -863,8 +992,26 @@
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4">
+        <v>11122019</v>
+      </c>
+      <c r="H4">
+        <v>12122022</v>
+      </c>
+      <c r="I4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -874,8 +1021,26 @@
       <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5">
+        <v>11122021</v>
+      </c>
+      <c r="H5">
+        <v>12122022</v>
+      </c>
+      <c r="I5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -885,8 +1050,26 @@
       <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6">
+        <v>11122020</v>
+      </c>
+      <c r="H6">
+        <v>12122022</v>
+      </c>
+      <c r="I6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -896,8 +1079,26 @@
       <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7">
+        <v>11122019</v>
+      </c>
+      <c r="H7">
+        <v>12122022</v>
+      </c>
+      <c r="I7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
@@ -907,8 +1108,26 @@
       <c r="C8" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8">
+        <v>11122021</v>
+      </c>
+      <c r="H8">
+        <v>12122022</v>
+      </c>
+      <c r="I8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -918,8 +1137,26 @@
       <c r="C9" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9">
+        <v>11122020</v>
+      </c>
+      <c r="H9">
+        <v>12122022</v>
+      </c>
+      <c r="I9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -928,6 +1165,24 @@
       </c>
       <c r="C10" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10">
+        <v>11122019</v>
+      </c>
+      <c r="H10">
+        <v>12122022</v>
+      </c>
+      <c r="I10" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>